<commit_message>
remove progress and opmize article
</commit_message>
<xml_diff>
--- a/cfg/article_cfg.xlsx
+++ b/cfg/article_cfg.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\DrunkFrog\cfg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Emanon\cfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD37B735-7759-4D9C-AB9A-1FCF3445B60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39EBF36-4BC3-4C45-998D-3F86AA7D89D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -105,6 +105,42 @@
   </si>
   <si>
     <t>网页地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文章名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如无必要，勿增实体</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色设计：无聊猿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>占领模式战场规则</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>局内派对点奖励规则</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>枪械后坐力规则</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>战令通行证功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂游戏系统设计与“涌现”理论</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -513,7 +549,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -550,6 +586,9 @@
       <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
@@ -561,6 +600,9 @@
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
@@ -572,6 +614,9 @@
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
@@ -583,7 +628,9 @@
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
@@ -596,7 +643,9 @@
       <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
@@ -609,7 +658,9 @@
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
@@ -622,7 +673,9 @@
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
@@ -635,7 +688,9 @@
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
@@ -648,7 +703,9 @@
       <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
@@ -661,7 +718,9 @@
       <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>